<commit_message>
Updated open office and closed to be unique
Based on some research I adjusted the density and EPD down for closed
offices and up for private offices.  I don't know that my values are
correct, but they are better than they were when they were the same as
each other. In the end, this is a starting point and modelers can adjust
based on their specific building design.
</commit_message>
<xml_diff>
--- a/space_types/supporting docs/MultiSpaceTypeOfficeWorksheet.xlsx
+++ b/space_types/supporting docs/MultiSpaceTypeOfficeWorksheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="180" windowWidth="27795" windowHeight="12525" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="240" windowWidth="18720" windowHeight="7185" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -12,11 +12,12 @@
     <sheet name="Proposed Space Type 2004" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="123">
   <si>
     <t>Office Space Type breakdown in TSD documents.</t>
   </si>
@@ -321,61 +322,70 @@
     <t>BreakRoom</t>
   </si>
   <si>
-    <t>OfficePrivate</t>
+    <t>note: I'm currently using0.96 cfm/sqft (TSD's use exhaust instead and have no ventilation)</t>
+  </si>
+  <si>
+    <t>It seems like small and medium office should have different occupancy and load densities from each other</t>
+  </si>
+  <si>
+    <t>Should Elevator be a space type, and if so what should it look like</t>
+  </si>
+  <si>
+    <t>cfm person total</t>
+  </si>
+  <si>
+    <t>cfm area total</t>
+  </si>
+  <si>
+    <t>(ref sm office schedule adjusted peak people - ref)</t>
+  </si>
+  <si>
+    <t>(TSD sm office schedule adjusted peak people - ref)</t>
+  </si>
+  <si>
+    <t>Office Infil Quarter On</t>
+  </si>
+  <si>
+    <t>sources for data are ref building, TSD, and standards spreadsheet dat</t>
+  </si>
+  <si>
+    <t>Look at infiltration for different vintages. Here is what spreadhseet shows</t>
+  </si>
+  <si>
+    <t>Pre 1980</t>
+  </si>
+  <si>
+    <t>1980-2004</t>
+  </si>
+  <si>
+    <t>2009 1-3</t>
+  </si>
+  <si>
+    <t>2009 4-8</t>
+  </si>
+  <si>
+    <t>(ft^3/min*ft^2 ext)</t>
+  </si>
+  <si>
+    <t>Not sure of the source of these values.</t>
+  </si>
+  <si>
+    <t>On Demand</t>
+  </si>
+  <si>
+    <t>Talking to Shanti, may make sense to slightly raise the people and plug load density for open office, and increase the lighting for closed. Look at 62.1</t>
+  </si>
+  <si>
+    <t>OfficeOpen</t>
+  </si>
+  <si>
+    <t>Good link from wbdg.org</t>
+  </si>
+  <si>
+    <t>http://www.wbdg.org/design/office_st.php</t>
   </si>
   <si>
     <t>OfficeClosed</t>
-  </si>
-  <si>
-    <t>note: I'm currently using0.96 cfm/sqft (TSD's use exhaust instead and have no ventilation)</t>
-  </si>
-  <si>
-    <t>It seems like small and medium office should have different occupancy and load densities from each other</t>
-  </si>
-  <si>
-    <t>Should Elevator be a space type, and if so what should it look like</t>
-  </si>
-  <si>
-    <t>cfm person total</t>
-  </si>
-  <si>
-    <t>cfm area total</t>
-  </si>
-  <si>
-    <t>(ref sm office schedule adjusted peak people - ref)</t>
-  </si>
-  <si>
-    <t>(TSD sm office schedule adjusted peak people - ref)</t>
-  </si>
-  <si>
-    <t>Office Infil Quarter On</t>
-  </si>
-  <si>
-    <t>sources for data are ref building, TSD, and standards spreadsheet dat</t>
-  </si>
-  <si>
-    <t>Look at infiltration for different vintages. Here is what spreadhseet shows</t>
-  </si>
-  <si>
-    <t>Pre 1980</t>
-  </si>
-  <si>
-    <t>1980-2004</t>
-  </si>
-  <si>
-    <t>2009 1-3</t>
-  </si>
-  <si>
-    <t>2009 4-8</t>
-  </si>
-  <si>
-    <t>(ft^3/min*ft^2 ext)</t>
-  </si>
-  <si>
-    <t>Not sure of the source of these values.</t>
-  </si>
-  <si>
-    <t>On Demand</t>
   </si>
 </sst>
 </file>
@@ -638,7 +648,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -796,15 +806,6 @@
     <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -818,6 +819,18 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="2" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1128,7 +1141,7 @@
   <dimension ref="A1:M87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B89" sqref="B89"/>
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1513,13 +1526,13 @@
       <c r="J21" s="21"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="82" t="s">
+      <c r="A22" s="79" t="s">
         <v>45</v>
       </c>
       <c r="J22" s="21"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="83" t="s">
+      <c r="A23" s="80" t="s">
         <v>43</v>
       </c>
       <c r="J23" s="21"/>
@@ -3394,10 +3407,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:R61"/>
+  <dimension ref="A2:R64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3410,7 +3423,7 @@
   <sheetData>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -3428,7 +3441,7 @@
       <c r="B5" s="17"/>
       <c r="C5" s="18">
         <f>M22</f>
-        <v>172.3</v>
+        <v>173.00000000000003</v>
       </c>
       <c r="D5" s="18"/>
       <c r="E5" s="18"/>
@@ -3453,20 +3466,20 @@
       <c r="E6" s="7"/>
       <c r="F6" s="44"/>
       <c r="G6" s="44"/>
-      <c r="H6" s="81" t="s">
+      <c r="H6" s="92" t="s">
         <v>42</v>
       </c>
-      <c r="I6" s="81"/>
+      <c r="I6" s="92"/>
       <c r="J6" s="10"/>
       <c r="K6" s="41"/>
       <c r="M6" s="55"/>
       <c r="N6" s="43"/>
       <c r="O6" s="43"/>
       <c r="P6" s="43"/>
-      <c r="Q6" s="79" t="s">
+      <c r="Q6" s="90" t="s">
         <v>75</v>
       </c>
-      <c r="R6" s="80"/>
+      <c r="R6" s="91"/>
     </row>
     <row r="7" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="45" t="s">
@@ -3494,7 +3507,7 @@
       <c r="I7" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="J7" s="91" t="s">
+      <c r="J7" s="88" t="s">
         <v>54</v>
       </c>
       <c r="K7" s="29" t="s">
@@ -3521,13 +3534,13 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="74" t="s">
-        <v>101</v>
+        <v>122</v>
       </c>
       <c r="B8" s="49">
         <v>0.15</v>
       </c>
-      <c r="C8" s="9">
-        <v>5</v>
+      <c r="C8" s="89">
+        <v>4.75</v>
       </c>
       <c r="D8" s="78">
         <v>0.85</v>
@@ -3535,11 +3548,12 @@
       <c r="E8" s="78" t="s">
         <v>97</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="89">
         <v>1.1000000000000001</v>
       </c>
-      <c r="G8" s="9">
-        <v>0.87</v>
+      <c r="G8" s="89">
+        <f>0.87*0.95</f>
+        <v>0.82650000000000001</v>
       </c>
       <c r="H8" s="9">
         <v>20</v>
@@ -3549,15 +3563,15 @@
         <v>5.9499999999999997E-2</v>
       </c>
       <c r="K8" s="41" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="M8" s="55">
         <f t="shared" ref="M8:M20" si="0">(C8*B8*$F$5)/1000</f>
-        <v>15</v>
+        <v>14.25</v>
       </c>
       <c r="N8" s="70">
         <f>M8*D8</f>
-        <v>12.75</v>
+        <v>12.112499999999999</v>
       </c>
       <c r="O8" s="43">
         <f>F8*B8*$F$5</f>
@@ -3565,11 +3579,11 @@
       </c>
       <c r="P8" s="43">
         <f>G8*B8*$F$5</f>
-        <v>2610</v>
+        <v>2479.5</v>
       </c>
       <c r="Q8" s="43">
         <f>H8*C8</f>
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="R8" s="56">
         <f t="shared" ref="R8:R20" si="1">I8*B8*$F$5</f>
@@ -3578,13 +3592,13 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="74" t="s">
-        <v>102</v>
+        <v>119</v>
       </c>
       <c r="B9" s="49">
         <v>0.28999999999999998</v>
       </c>
-      <c r="C9" s="9">
-        <v>5</v>
+      <c r="C9" s="89">
+        <v>5.25</v>
       </c>
       <c r="D9" s="78">
         <v>0.85</v>
@@ -3592,11 +3606,12 @@
       <c r="E9" s="78" t="s">
         <v>97</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="89">
         <v>1.1000000000000001</v>
       </c>
-      <c r="G9" s="9">
-        <v>0.87</v>
+      <c r="G9" s="89">
+        <f>0.87*1.05</f>
+        <v>0.91349999999999998</v>
       </c>
       <c r="H9" s="9">
         <v>20</v>
@@ -3606,15 +3621,15 @@
         <v>5.9499999999999997E-2</v>
       </c>
       <c r="K9" s="41" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="M9" s="55">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>30.45</v>
       </c>
       <c r="N9" s="70">
         <f t="shared" ref="N9:N20" si="2">M9*D9</f>
-        <v>24.65</v>
+        <v>25.8825</v>
       </c>
       <c r="O9" s="43">
         <f t="shared" ref="O9:O20" si="3">F9*B9*$F$5</f>
@@ -3622,11 +3637,11 @@
       </c>
       <c r="P9" s="43">
         <f t="shared" ref="P9:P20" si="4">G9*B9*$F$5</f>
-        <v>5045.9999999999991</v>
+        <v>5298.2999999999993</v>
       </c>
       <c r="Q9" s="43">
         <f>H9*C9</f>
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="R9" s="56">
         <f t="shared" si="1"/>
@@ -3663,7 +3678,7 @@
         <v>5.9499999999999997E-2</v>
       </c>
       <c r="K10" s="41" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="M10" s="55">
         <f t="shared" si="0"/>
@@ -3719,7 +3734,7 @@
         <v>5.9499999999999997E-2</v>
       </c>
       <c r="K11" s="41" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="M11" s="55">
         <f t="shared" si="0"/>
@@ -3770,7 +3785,7 @@
         <v>5.9499999999999997E-2</v>
       </c>
       <c r="K12" s="41" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="M12" s="55">
         <f t="shared" si="0"/>
@@ -3827,7 +3842,7 @@
         <v>5.9499999999999997E-2</v>
       </c>
       <c r="K13" s="41" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="M13" s="55">
         <f t="shared" si="0"/>
@@ -3884,7 +3899,7 @@
         <v>5.9499999999999997E-2</v>
       </c>
       <c r="K14" s="41" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="M14" s="55">
         <f t="shared" si="0"/>
@@ -3935,7 +3950,7 @@
         <v>5.9499999999999997E-2</v>
       </c>
       <c r="K15" s="41" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="M15" s="55">
         <f t="shared" si="0"/>
@@ -3986,7 +4001,7 @@
         <v>5.9499999999999997E-2</v>
       </c>
       <c r="K16" s="41" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="M16" s="55">
         <f t="shared" si="0"/>
@@ -4043,7 +4058,7 @@
         <v>5.9499999999999997E-2</v>
       </c>
       <c r="K17" s="41" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="M17" s="55">
         <f t="shared" si="0"/>
@@ -4100,7 +4115,7 @@
         <v>5.9499999999999997E-2</v>
       </c>
       <c r="K18" s="41" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="M18" s="55">
         <f t="shared" si="0"/>
@@ -4157,7 +4172,7 @@
         <v>5.9499999999999997E-2</v>
       </c>
       <c r="K19" s="41" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="M19" s="55">
         <f t="shared" si="0"/>
@@ -4214,7 +4229,7 @@
         <v>5.9499999999999997E-2</v>
       </c>
       <c r="K20" s="41" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="M20" s="55">
         <f t="shared" si="0"/>
@@ -4270,7 +4285,7 @@
       </c>
       <c r="C22" s="51">
         <f>(M22/F5)*1000</f>
-        <v>8.615000000000002</v>
+        <v>8.6500000000000021</v>
       </c>
       <c r="D22" s="65"/>
       <c r="E22" s="65"/>
@@ -4280,11 +4295,11 @@
       </c>
       <c r="G22" s="9">
         <f>P22/$F$5</f>
-        <v>0.91535</v>
+        <v>0.92143999999999993</v>
       </c>
       <c r="H22" s="9">
         <f>Q22/C5</f>
-        <v>12.188334300638422</v>
+        <v>12.139017341040461</v>
       </c>
       <c r="I22" s="9">
         <f>R22/F5</f>
@@ -4294,15 +4309,15 @@
         <v>5.9499999999999997E-2</v>
       </c>
       <c r="K22" s="41" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="M22" s="60">
         <f t="shared" ref="M22:R22" si="6">SUM(M8:M20)</f>
-        <v>172.3</v>
+        <v>173.00000000000003</v>
       </c>
       <c r="N22" s="71">
         <f t="shared" si="6"/>
-        <v>89.800000000000011</v>
+        <v>90.39500000000001</v>
       </c>
       <c r="O22" s="61">
         <f t="shared" si="6"/>
@@ -4310,7 +4325,7 @@
       </c>
       <c r="P22" s="61">
         <f t="shared" si="6"/>
-        <v>18307</v>
+        <v>18428.8</v>
       </c>
       <c r="Q22" s="61">
         <f t="shared" si="6"/>
@@ -4369,7 +4384,7 @@
       </c>
       <c r="N24" s="23">
         <f>N22*1000/F5</f>
-        <v>4.4900000000000011</v>
+        <v>4.519750000000001</v>
       </c>
       <c r="O24" s="41" t="s">
         <v>94</v>
@@ -4411,7 +4426,7 @@
         <v>4.75</v>
       </c>
       <c r="O25" s="41" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="26" spans="1:18" s="41" customFormat="1" x14ac:dyDescent="0.25">
@@ -4447,7 +4462,7 @@
         <v>4.18</v>
       </c>
       <c r="O26" s="41" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
@@ -4491,7 +4506,7 @@
       </c>
       <c r="E32" s="44"/>
     </row>
-    <row r="33" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>3</v>
       </c>
@@ -4502,8 +4517,9 @@
         <v>88</v>
       </c>
       <c r="E33" s="44"/>
-    </row>
-    <row r="34" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="N33"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>4</v>
       </c>
@@ -4514,24 +4530,23 @@
         <v>88</v>
       </c>
       <c r="E34" s="44"/>
-    </row>
-    <row r="37" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="N34"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="73"/>
       <c r="B37" s="46" t="s">
-        <v>103</v>
-      </c>
-      <c r="D37" s="41"/>
-      <c r="E37" s="41"/>
-    </row>
-    <row r="39" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="N37"/>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B39" s="41" t="s">
         <v>85</v>
       </c>
       <c r="C39" s="41"/>
-      <c r="D39" s="41"/>
-      <c r="E39" s="41"/>
-    </row>
-    <row r="40" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="N39"/>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B40" s="52"/>
       <c r="C40" s="66" t="s">
         <v>89</v>
@@ -4542,10 +4557,11 @@
       <c r="E40" s="67" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="N40"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B41" s="55" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C41" s="76">
         <f>Q22</f>
@@ -4559,10 +4575,11 @@
         <f>H25*C25*F5/1000</f>
         <v>2648</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="N41"/>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B42" s="55" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C42" s="76">
         <f>R22</f>
@@ -4570,8 +4587,9 @@
       </c>
       <c r="D42" s="76"/>
       <c r="E42" s="77"/>
-    </row>
-    <row r="43" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="N42"/>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B43" s="60" t="s">
         <v>74</v>
       </c>
@@ -4587,102 +4605,116 @@
         <f>SUM(E41:E42)</f>
         <v>2648</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="N43"/>
+    </row>
+    <row r="44" spans="1:14" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B44" s="43"/>
       <c r="C44" s="43"/>
       <c r="D44" s="43"/>
       <c r="E44" s="43"/>
     </row>
-    <row r="46" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="74"/>
       <c r="B46" t="s">
-        <v>104</v>
-      </c>
-      <c r="D46" s="41"/>
-      <c r="E46" s="41"/>
+        <v>102</v>
+      </c>
       <c r="G46" s="41"/>
       <c r="H46" s="41"/>
       <c r="I46" s="41"/>
       <c r="J46" s="41"/>
       <c r="K46" s="41"/>
-    </row>
-    <row r="47" spans="1:11" s="41" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A49" s="75"/>
-      <c r="B49" t="s">
-        <v>105</v>
-      </c>
-      <c r="D49"/>
-      <c r="E49"/>
-      <c r="N49"/>
-    </row>
+      <c r="N46"/>
+    </row>
+    <row r="47" spans="1:14" s="86" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:14" s="86" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="86" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" s="86" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="86" t="s">
+        <v>120</v>
+      </c>
+      <c r="D49" s="86" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" s="41" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A52" s="90"/>
+      <c r="A52" s="75"/>
       <c r="B52" t="s">
-        <v>112</v>
-      </c>
-      <c r="F52" s="84"/>
-    </row>
-    <row r="53" spans="1:14" s="89" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="89" t="s">
-        <v>118</v>
-      </c>
-      <c r="F53" s="84"/>
-    </row>
-    <row r="54" spans="1:14" s="89" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F54" s="84"/>
-    </row>
-    <row r="55" spans="1:14" s="89" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C55" s="89" t="s">
-        <v>119</v>
-      </c>
-      <c r="F55" s="84"/>
-    </row>
-    <row r="56" spans="1:14" s="89" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C56" s="84" t="s">
+        <v>103</v>
+      </c>
+      <c r="D52"/>
+      <c r="E52"/>
+      <c r="N52"/>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A55" s="87"/>
+      <c r="B55" t="s">
+        <v>110</v>
+      </c>
+      <c r="F55" s="81"/>
+    </row>
+    <row r="56" spans="1:14" s="86" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="86" t="s">
+        <v>116</v>
+      </c>
+      <c r="F56" s="81"/>
+    </row>
+    <row r="57" spans="1:14" s="86" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F57" s="81"/>
+    </row>
+    <row r="58" spans="1:14" s="86" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C58" s="86" t="s">
         <v>117</v>
       </c>
-      <c r="F56" s="84"/>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B57" s="44" t="s">
-        <v>113</v>
-      </c>
-      <c r="C57" s="85">
-        <v>0.22320000000000001</v>
-      </c>
-      <c r="D57" s="86"/>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B58" s="44" t="s">
-        <v>114</v>
-      </c>
-      <c r="C58" s="87">
-        <v>0.22320000000000001</v>
-      </c>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B59" s="44">
-        <v>2004</v>
-      </c>
-      <c r="C59" s="88">
-        <v>5.9499999999999997E-2</v>
-      </c>
+      <c r="F58" s="81"/>
+    </row>
+    <row r="59" spans="1:14" s="86" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C59" s="81" t="s">
+        <v>115</v>
+      </c>
+      <c r="F59" s="81"/>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B60" s="44" t="s">
-        <v>115</v>
-      </c>
-      <c r="C60" s="88">
-        <v>5.9499999999999997E-2</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="C60" s="82">
+        <v>0.22320000000000001</v>
+      </c>
+      <c r="D60" s="83"/>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B61" s="44" t="s">
-        <v>116</v>
-      </c>
-      <c r="C61" s="89">
+        <v>112</v>
+      </c>
+      <c r="C61" s="84">
+        <v>0.22320000000000001</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B62" s="44">
+        <v>2004</v>
+      </c>
+      <c r="C62" s="85">
+        <v>5.9499999999999997E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B63" s="44" t="s">
+        <v>113</v>
+      </c>
+      <c r="C63" s="85">
+        <v>5.9499999999999997E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B64" s="44" t="s">
+        <v>114</v>
+      </c>
+      <c r="C64" s="86">
         <v>4.4600000000000001E-2</v>
       </c>
     </row>

</xml_diff>